<commit_message>
Fix incorrect test value in test_cross_sheet_join.xlsx: 'Charles' -> 'Carol'.
</commit_message>
<xml_diff>
--- a/contrib/format-excel/src/test/resources/excel/test_cross_sheet_join.xlsx
+++ b/contrib/format-excel/src/test/resources/excel/test_cross_sheet_join.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="customers" sheetId="1" state="visible" r:id="rId2"/>
@@ -35,7 +35,7 @@
     <t xml:space="preserve">Bob</t>
   </si>
   <si>
-    <t xml:space="preserve">Charles</t>
+    <t xml:space="preserve">Carol</t>
   </si>
   <si>
     <t xml:space="preserve">Dave</t>
@@ -159,11 +159,11 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -231,11 +231,11 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>